<commit_message>
weekly report 5 document
</commit_message>
<xml_diff>
--- a/static/DTC_Gantt_Chart.xlsx
+++ b/static/DTC_Gantt_Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="202" documentId="13_ncr:1_{82601C84-680F-416C-8597-3278F6EF5C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74FCAC8B-DECF-4D24-A89C-8A12D43D6957}"/>
+  <xr:revisionPtr revIDLastSave="216" documentId="13_ncr:1_{82601C84-680F-416C-8597-3278F6EF5C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1DC9C4A-1463-4DCC-B357-DAB596EB20D1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -794,6 +794,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1027,8 +1031,8 @@
   </sheetPr>
   <dimension ref="B1:AQ17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1344,7 +1348,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" s="8">
         <v>0.5</v>
@@ -1368,7 +1372,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="8">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="S9" s="22"/>
     </row>
@@ -1383,13 +1387,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F10" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10" s="22"/>
     </row>
@@ -1425,13 +1429,13 @@
         <v>3</v>
       </c>
       <c r="E12" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F12" s="7">
         <v>0</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="S12" s="22"/>
     </row>
@@ -1446,13 +1450,13 @@
         <v>4</v>
       </c>
       <c r="E13" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F13" s="7">
         <v>0</v>
       </c>
       <c r="G13" s="8">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S13" s="22"/>
     </row>
@@ -1612,7 +1616,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="51" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="67" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
update landing page, api spec, gantt chart, remove old logo
</commit_message>
<xml_diff>
--- a/static/DTC_Gantt_Chart.xlsx
+++ b/static/DTC_Gantt_Chart.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="240" documentId="13_ncr:1_{82601C84-680F-416C-8597-3278F6EF5C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC72A49C-168B-4AEF-BF69-88240C99EEF6}"/>
+  <xr:revisionPtr revIDLastSave="255" documentId="13_ncr:1_{82601C84-680F-416C-8597-3278F6EF5C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{142473ED-9570-4BD5-BED7-2EE7471BFB61}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1407,10 +1407,10 @@
         <v>7</v>
       </c>
       <c r="F11" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G11" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S11" s="22"/>
     </row>
@@ -1428,10 +1428,10 @@
         <v>4</v>
       </c>
       <c r="F12" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G12" s="8">
-        <v>0.66</v>
+        <v>1</v>
       </c>
       <c r="S12" s="22"/>
     </row>
@@ -1449,10 +1449,10 @@
         <v>5</v>
       </c>
       <c r="F13" s="7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G13" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S13" s="22"/>
     </row>
@@ -1470,10 +1470,10 @@
         <v>8</v>
       </c>
       <c r="F14" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G14" s="8">
-        <v>0.33</v>
+        <v>0.66</v>
       </c>
       <c r="S14" s="22"/>
     </row>

</xml_diff>